<commit_message>
Scripting DPLKINV001-013, Update Function Sidebar Menu, and Spying Browser Object
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-013 - Setup Emiten Investasi - General Tambah, Ubah, View Detil & Hapus Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-013 - Setup Emiten Investasi - General Tambah, Ubah, View Detil & Hapus Data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C57D95F-94C8-4A1F-83F9-E07260BFF1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPLKINV001" sheetId="2" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -22,9 +28,6 @@
     <t>SIDEBAR_SUBMENU</t>
   </si>
   <si>
-    <t>SIDEBAR_SUBMENU_SUBMENU</t>
-  </si>
-  <si>
     <t>RUN</t>
   </si>
   <si>
@@ -46,30 +49,6 @@
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>TEXT1</t>
-  </si>
-  <si>
-    <t>TEXT2</t>
-  </si>
-  <si>
-    <t>TEXT3</t>
-  </si>
-  <si>
-    <t>TEXT4</t>
-  </si>
-  <si>
-    <t>TEXT5</t>
-  </si>
-  <si>
-    <t>TEXT6</t>
-  </si>
-  <si>
-    <t>TEXT7</t>
-  </si>
-  <si>
-    <t>TEXT8</t>
-  </si>
-  <si>
     <t>Normal - Investasi - General</t>
   </si>
   <si>
@@ -100,12 +79,6 @@
     <t>Hapus Data Dapat dilakukan dengan baik</t>
   </si>
   <si>
-    <t>TEXT9</t>
-  </si>
-  <si>
-    <t>TEXT10</t>
-  </si>
-  <si>
     <t>INV001-013</t>
   </si>
   <si>
@@ -122,13 +95,179 @@
   </si>
   <si>
     <t>Hapus Setup Emiten</t>
+  </si>
+  <si>
+    <t>PREPARATION</t>
+  </si>
+  <si>
+    <t>Username : Putri;
+Password : bni1234/;
+Kode Emiten : -;
+Group Emiten : BCA Group;
+Jenis Emiten : Swasta;
+Nama Emiten : Tester;
+Ticker : Test;
+Keterangan : INV.SET.013;
+Sektor : 4- - Keuangan;
+Sub Sektor : Keuangan / Perbankan;
+Kode BI : 014 - Bank BCA;
+Alamat : Jalan Testing;
+Kota : Jakarta;
+Kode Post : 99999;
+Nama Kontak : Test;
+NPWP : 123456789;
+Telepon : 0123456789;
+Fax : 99999999;
+Email : test@gmail.com;
+No Rekening : 01;
+Bank : 014 - Bank BCA;
+Cabang : Bekasi;
+No. Rekening : 12131313131;
+Pemilik Rekening : Tester;
+Default : Ya</t>
+  </si>
+  <si>
+    <t>Username : Putri;
+Password : bni1234/;
+Kode Emiten : E0062</t>
+  </si>
+  <si>
+    <t>Username : Putri;
+Password : bni1234/;
+No. Rekening : 12345678</t>
+  </si>
+  <si>
+    <t>KODE_EMITEN</t>
+  </si>
+  <si>
+    <t>GROUP_EMITEN</t>
+  </si>
+  <si>
+    <t>JENIS_EMITEN</t>
+  </si>
+  <si>
+    <t>NAMA_EMITEN</t>
+  </si>
+  <si>
+    <t>TICKER</t>
+  </si>
+  <si>
+    <t>KETERANGAN</t>
+  </si>
+  <si>
+    <t>SEKTOR</t>
+  </si>
+  <si>
+    <t>SUB_SEKTOR</t>
+  </si>
+  <si>
+    <t>KODE_BI</t>
+  </si>
+  <si>
+    <t>ALAMAT</t>
+  </si>
+  <si>
+    <t>KOTA</t>
+  </si>
+  <si>
+    <t>KODE_POS</t>
+  </si>
+  <si>
+    <t>NAMA_KONTRAK</t>
+  </si>
+  <si>
+    <t>NPWP</t>
+  </si>
+  <si>
+    <t>TELEPON</t>
+  </si>
+  <si>
+    <t>FAX</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>STATUS_REGISTER</t>
+  </si>
+  <si>
+    <t>KETERANGAN_REGISTER</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>BANK</t>
+  </si>
+  <si>
+    <t>CABANG</t>
+  </si>
+  <si>
+    <t>NO_REKENING</t>
+  </si>
+  <si>
+    <t>PEMILIK_REKENING</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>BCA GROUP</t>
+  </si>
+  <si>
+    <t>SWASTA</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>INV.SET.013</t>
+  </si>
+  <si>
+    <t>4 : Keuangan</t>
+  </si>
+  <si>
+    <t>Keuangan / Perbankan</t>
+  </si>
+  <si>
+    <t>014 : Bank BCA</t>
+  </si>
+  <si>
+    <t>Jalan Testing</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>0 : Pending Register</t>
+  </si>
+  <si>
+    <t>Testing Add Setup Emiten</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>Bekasi</t>
+  </si>
+  <si>
+    <t>Ya</t>
+  </si>
+  <si>
+    <t>Tester 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +300,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,10 +326,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -208,8 +356,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,11 +668,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,167 +681,296 @@
     <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="16" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="12" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="32.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="390" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" s="1">
+        <v>99999</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>99999999</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>12131313131</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="J3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-    </row>
-    <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="4"/>
       <c r="L3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="O3" s="7"/>
+      <c r="O3" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
@@ -694,85 +978,96 @@
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="4"/>
       <c r="L4" s="5"/>
       <c r="M4" s="8"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="7"/>
+      <c r="O4" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
+      <c r="AH4" s="1">
+        <v>12345678</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="G5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="4"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="7"/>
+      <c r="O5" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
@@ -780,19 +1075,22 @@
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="AB2" r:id="rId1" xr:uid="{31C0F554-089B-49B3-A953-B5EC5F01C8A3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>